<commit_message>
Implement sign-up and login functionality with corresponding page objects
</commit_message>
<xml_diff>
--- a/Harsha_Incubyte_Test_Cases.xlsx
+++ b/Harsha_Incubyte_Test_Cases.xlsx
@@ -34,23 +34,18 @@
     <t>TC001</t>
   </si>
   <si>
-    <t>Verify Successful Account Creation (Sign-Up)</t>
+    <t>Verify Successful Account Creation</t>
   </si>
   <si>
-    <t>User is on the Magento sign-up page.</t>
+    <t>User is on the sign-up page</t>
   </si>
   <si>
-    <t>1. Navigate to the Magento sign-up page.
-2. Enter valid details in the required fields:
-- First Name
-- Last Name
-- Email
-- Password
-- Confirm Password
-3. Click the “Create an Account” button.</t>
+    <t>1. Navigate to sign-up page.
+2. Enter valid user details.
+3. Click “Create Account.”</t>
   </si>
   <si>
-    <t>The account is successfully created, and a confirmation message along with redirection to the account dashboard is displayed.</t>
+    <t>User redirected and confirmation message displayed along with dashboard.</t>
   </si>
   <si>
     <t>Pass</t>
@@ -59,18 +54,18 @@
     <t>TC002</t>
   </si>
   <si>
-    <t>Verify Successful Login with Created Account (Sign-In)</t>
+    <t>Verify Successful Login</t>
   </si>
   <si>
-    <t>Account successfully created from TC001.</t>
+    <t>Account created from TC001</t>
   </si>
   <si>
-    <t>1. Navigate to the Magento login page.
-2. Enter valid credentials (email and password from account created in TC001).
+    <t>1. Navigate to login page.
+2. Enter valid credentials.
 3. Click “Sign In.”</t>
   </si>
   <si>
-    <t>User successfully logs in, and account dashboard is displayed.</t>
+    <t>User successfully logs in and sees account dashboard.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Add negative test cases
</commit_message>
<xml_diff>
--- a/Harsha_Incubyte_Test_Cases.xlsx
+++ b/Harsha_Incubyte_Test_Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -40,12 +40,13 @@
     <t>User is on the sign-up page</t>
   </si>
   <si>
-    <t>1. Navigate to sign-up page.
-2. Enter valid user details.
-3. Click “Create Account.”</t>
+    <t>1. Given user is on sign-up page.
+2. When user enters valid user details
+.
+3. Then user clicks "Create Account."</t>
   </si>
   <si>
-    <t>User redirected and confirmation message displayed along with dashboard.</t>
+    <t>User should see a confirmation message and be redirected to the account dashboard.</t>
   </si>
   <si>
     <t>Pass</t>
@@ -60,12 +61,76 @@
     <t>Account created from TC001</t>
   </si>
   <si>
-    <t>1. Navigate to login page.
-2. Enter valid credentials.
-3. Click “Sign In.”</t>
+    <t>1. Given user is on login page.
+2. When user enters valid credentials.
+3. Then user clicks "Sign In."</t>
   </si>
   <si>
-    <t>User successfully logs in and sees account dashboard.</t>
+    <t>User should successfully log in and see the account dashboard.</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Invalid Login Attempt	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on the login page	</t>
+  </si>
+  <si>
+    <t>1. Given user navigates to the login page.
+2. When user enters invalid credentials email and password.
+3. And clicks Sign In.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see an error message indicating incorrect credentials.	</t>
+  </si>
+  <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Logout Functionality	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is logged into their account	</t>
+  </si>
+  <si>
+    <t>1. Given user is logged into their account
+.
+2. When user clicks on the logout button.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be redirected to the sign-out page and no longer see the account dashboard.	</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Duplicate Email Check	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on the sign-up page	</t>
+  </si>
+  <si>
+    <t>1. Given user is on sign-up page.
+2. When user enters valid details first name, last name, existing email, and password.
+3. And clicks Create Account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see an error message indicating the email is already in use.	</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Password Strength Validation	</t>
+  </si>
+  <si>
+    <t>1. Given user is on sign-up page.
+2. When user enters first name, last name, email, and weak password.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should see an error message indicating the password does not meet strength requirements.	</t>
   </si>
 </sst>
 </file>
@@ -129,7 +194,7 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -492,12 +557,24 @@
       <c r="Z3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -520,12 +597,24 @@
       <c r="Z4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -548,12 +637,24 @@
       <c r="Z5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
@@ -576,12 +677,24 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="A7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -604,7 +717,7 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="7"/>
+      <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>

</xml_diff>